<commit_message>
fix: refactor to input_path(), fix merging paths
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_C.xlsx
+++ b/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="C.1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">KEY</t>
@@ -168,11 +165,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -207,25 +204,25 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="211" zoomScaleNormal="211" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -233,10 +230,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,10 +241,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,10 +252,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,10 +263,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -277,10 +274,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,10 +285,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,10 +296,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,10 +307,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>